<commit_message>
JEE Vehicle Ordering Server aus dem Boden gestampft (README!)
- Servicenamen sind jetzt im Plural (ist in der Schnittstellendefinition
festgehalten); z.B. "services/orders" statt "services/order" um alle
Bestellungen aufzulisten

- POSTet man einen neuen Kunden oder Bestellung, muss das XML wie das
beim GET erhaltene aussehen; dabei ist die ID des Kunden/Bestellung egal
und wird ignoriert, wird jedoch trotzdem von JAXP benötigt; ACHTUNG: die
IDs der Kindelemente, z.B des Models, muss jedoch stimmen!

- ich habe sämtliche Schnittstellen erfolgreich mit RESTClient getestet
</commit_message>
<xml_diff>
--- a/doc/Vehicle Ordering REST-Schnittstelle.xlsx
+++ b/doc/Vehicle Ordering REST-Schnittstelle.xlsx
@@ -45,36 +45,6 @@
     <t>application/xml</t>
   </si>
   <si>
-    <t>vehicle-ordering/services/type</t>
-  </si>
-  <si>
-    <t>vehicle-ordering/services/type/id</t>
-  </si>
-  <si>
-    <t>vehicle-ordering/services/model?type=id</t>
-  </si>
-  <si>
-    <t>vehicle-ordering/services/model/id</t>
-  </si>
-  <si>
-    <t>vehicle-ordering/services/customer?first=name&amp;last=name</t>
-  </si>
-  <si>
-    <t>vehicle-ordering/services/customer/id</t>
-  </si>
-  <si>
-    <t>vehicle-ordering/services/order?first=name&amp;last=name&amp;model=id</t>
-  </si>
-  <si>
-    <t>vehicle-ordering/services/order/id</t>
-  </si>
-  <si>
-    <t>vehicle-ordering/services/customer</t>
-  </si>
-  <si>
-    <t>vehicle-ordering/services/order</t>
-  </si>
-  <si>
     <t>Liste aller Typen</t>
   </si>
   <si>
@@ -109,6 +79,36 @@
   </si>
   <si>
     <t>Anlegen einer Bestellung; XML muss der aus Schnittstelle 8 entsprechen</t>
+  </si>
+  <si>
+    <t>vehicle-ordering/services/types</t>
+  </si>
+  <si>
+    <t>vehicle-ordering/services/types/id</t>
+  </si>
+  <si>
+    <t>vehicle-ordering/services/models?type=id</t>
+  </si>
+  <si>
+    <t>vehicle-ordering/services/models/id</t>
+  </si>
+  <si>
+    <t>vehicle-ordering/services/customers?first=name&amp;last=name</t>
+  </si>
+  <si>
+    <t>vehicle-ordering/services/customers/id</t>
+  </si>
+  <si>
+    <t>vehicle-ordering/services/orders?first=name&amp;last=name&amp;model=id</t>
+  </si>
+  <si>
+    <t>vehicle-ordering/services/orders/id</t>
+  </si>
+  <si>
+    <t>vehicle-ordering/services/customers</t>
+  </si>
+  <si>
+    <t>vehicle-ordering/services/orders</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +502,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -517,7 +517,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -528,16 +528,16 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -548,16 +548,16 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -568,16 +568,16 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -588,16 +588,16 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -608,7 +608,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>6</v>
@@ -617,7 +617,7 @@
         <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -628,7 +628,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>6</v>
@@ -637,7 +637,7 @@
         <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -648,7 +648,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>6</v>
@@ -657,7 +657,7 @@
         <v>7</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -668,7 +668,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>6</v>
@@ -677,7 +677,7 @@
         <v>7</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -688,7 +688,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>7</v>
@@ -697,7 +697,7 @@
         <v>8</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -708,7 +708,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>7</v>
@@ -717,7 +717,7 @@
         <v>8</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>